<commit_message>
BE LTD Axis UTR Process Commit
</commit_message>
<xml_diff>
--- a/BE_LTD_Axis_UTR/Data/Config.xlsx
+++ b/BE_LTD_Axis_UTR/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL\Documents\UiPath\BE_LTD_Axis_UTR\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB674F20-F475-4B8F-AD09-5236B6FEF1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDB2402-CDC9-4DA4-9664-67610EB874DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -100,9 +100,6 @@
     <t>TotalAmount</t>
   </si>
   <si>
-    <t>(INR) \d+(,\d+)*(\.\d+)</t>
-  </si>
-  <si>
     <t>CurrentDate</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
     <t>@SQL=urn:schemas:httpmail:subject LIKE '%Vendor_Payments%'</t>
   </si>
   <si>
-    <t>@SQL=urn:schemas:httpmail:fromname LIKE '%Straight2axis@axisbank.com%'</t>
-  </si>
-  <si>
     <t>C:\Users\BRADSOL\Documents\GitHub\brad-uipath\BRADSOL_Reusable_Tasks\Send Mail\Send Mail.xaml</t>
   </si>
   <si>
@@ -413,6 +407,39 @@
   </si>
   <si>
     <t>Hello Team,&lt;p&gt;This is to notify you that our BOT couldn’t find  attachments for attached mails the process of "Axis UTR Automation".&lt;p&gt;Thanks &amp; Regards,&lt;p&gt;BE Ltd.</t>
+  </si>
+  <si>
+    <t>\d+(,\d+)*(\.\d+)</t>
+  </si>
+  <si>
+    <t>VendorCode</t>
+  </si>
+  <si>
+    <t>(?&lt;=Beneficiary Code :)(.*)(?= Payment)</t>
+  </si>
+  <si>
+    <t>ValidationFailedPDFPath</t>
+  </si>
+  <si>
+    <t>C:\Users\BRADSOL\Documents\UiPath\BE_LTD_Axis_UTR\Data\Temp\ValidationFailedPDF\</t>
+  </si>
+  <si>
+    <t>CurrentDateMailsNotFoundSubject</t>
+  </si>
+  <si>
+    <t>CurrentDateMailsNotFoundBody</t>
+  </si>
+  <si>
+    <t>BE_LTD Axis Process- Axis Bank Current Date Emails not found</t>
+  </si>
+  <si>
+    <t>Hello Team,&lt;p&gt;This is to notify you that our BOT couldn’t find any Axis Bank current date emails for the process of "Axis UTR Automation".&lt;p&gt;Thanks &amp; Regards,&lt;p&gt;BE Ltd.</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>@SQL=urn:schemas:httpmail:fromname LIKE '%Straight2axis@axisbank.com%' AND urn:schemas:httpmail:datereceived &gt;= '</t>
   </si>
 </sst>
 </file>
@@ -472,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -483,6 +510,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z972"/>
+  <dimension ref="A1:Z967"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -861,7 +889,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -869,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -877,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -901,7 +929,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -933,135 +961,135 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
         <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
         <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
         <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
@@ -1074,30 +1102,51 @@
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33">
+        <v>-145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2017,11 +2066,6 @@
     <row r="965" ht="14.25" customHeight="1"/>
     <row r="966" ht="14.25" customHeight="1"/>
     <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2031,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z986"/>
+  <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2081,131 +2125,131 @@
     </row>
     <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -2213,98 +2257,98 @@
     </row>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
         <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28">
         <v>587</v>
@@ -2312,62 +2356,76 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
         <v>91</v>
-      </c>
-      <c r="B29" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" t="s">
         <v>110</v>
       </c>
-      <c r="B35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+    </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3315,8 +3373,6 @@
     <row r="982" ht="14.25" customHeight="1"/>
     <row r="983" ht="14.25" customHeight="1"/>
     <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3344,13 +3400,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>